<commit_message>
trainings: added [training_type] to the XLSX export.
</commit_message>
<xml_diff>
--- a/htdocs/assets/trainings.xlsx
+++ b/htdocs/assets/trainings.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t xml:space="preserve">№</t>
   </si>
@@ -76,6 +76,9 @@
     <t xml:space="preserve">Должность</t>
   </si>
   <si>
+    <t xml:space="preserve">Вид обучения</t>
+  </si>
+  <si>
     <t xml:space="preserve">Фото</t>
   </si>
   <si>
@@ -107,6 +110,9 @@
   </si>
   <si>
     <t xml:space="preserve">21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22</t>
   </si>
   <si>
     <t xml:space="preserve">23</t>
@@ -375,7 +381,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="Q1" activeCellId="0" sqref="Q1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="U3" activeCellId="0" sqref="U3"/>
+      <selection pane="bottomRight" activeCell="R3" activeCellId="0" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -395,13 +401,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="4" width="11.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="3" width="33.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="3" width="30.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="3" width="20.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="4" width="5.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="3" width="39.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="3" width="19.65"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="64" min="23" style="5" width="8.5"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1013" min="65" style="6" width="8.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1014" style="0" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="3" width="20.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="4" width="5.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="3" width="39.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="3" width="19.65"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="65" min="24" style="5" width="8.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="66" style="6" width="8.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1015" style="0" width="10.5"/>
   </cols>
   <sheetData>
     <row r="1" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -426,7 +432,7 @@
       <c r="T1" s="9"/>
       <c r="U1" s="9"/>
       <c r="V1" s="9"/>
-      <c r="ALZ1" s="0"/>
+      <c r="W1" s="9"/>
       <c r="AMA1" s="0"/>
       <c r="AMB1" s="0"/>
       <c r="AMC1" s="0"/>
@@ -496,12 +502,15 @@
       <c r="S2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12" t="s">
+      <c r="T2" s="12" t="s">
         <v>19</v>
       </c>
+      <c r="U2" s="12"/>
       <c r="V2" s="12" t="s">
         <v>20</v>
+      </c>
+      <c r="W2" s="12" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -545,36 +554,39 @@
         <v>13</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O3" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P3" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q3" s="14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="R3" s="14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="S3" s="14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="T3" s="14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="U3" s="14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="V3" s="14" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="W3" s="14" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="T2:U2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
trainings: added [activity_type] column.
</commit_message>
<xml_diff>
--- a/htdocs/assets/trainings.xlsx
+++ b/htdocs/assets/trainings.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t xml:space="preserve">№</t>
   </si>
@@ -88,6 +88,9 @@
     <t xml:space="preserve">Руководитель</t>
   </si>
   <si>
+    <t xml:space="preserve">Вид активности</t>
+  </si>
+  <si>
     <t xml:space="preserve">14</t>
   </si>
   <si>
@@ -116,6 +119,9 @@
   </si>
   <si>
     <t xml:space="preserve">23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24</t>
   </si>
 </sst>
 </file>
@@ -377,11 +383,11 @@
   <dimension ref="A1:AMJ3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="Q4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="Q1" activeCellId="0" sqref="Q1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="R3" activeCellId="0" sqref="R3"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -405,7 +411,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="4" width="5.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="3" width="39.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="3" width="19.65"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="65" min="24" style="5" width="8.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="3" width="20.16"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="65" min="25" style="5" width="8.5"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="66" style="6" width="8.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1015" style="0" width="10.5"/>
   </cols>
@@ -433,6 +440,7 @@
       <c r="U1" s="9"/>
       <c r="V1" s="9"/>
       <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
       <c r="AMA1" s="0"/>
       <c r="AMB1" s="0"/>
       <c r="AMC1" s="0"/>
@@ -512,6 +520,9 @@
       <c r="W2" s="12" t="s">
         <v>21</v>
       </c>
+      <c r="X2" s="12" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="13" t="n">
@@ -554,34 +565,37 @@
         <v>13</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O3" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P3" s="14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q3" s="14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R3" s="14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="S3" s="14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="T3" s="14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U3" s="14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="V3" s="14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="W3" s="14" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="X3" s="14" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>